<commit_message>
fixing the restaurants limit in the search after skipping the chain restauants results
</commit_message>
<xml_diff>
--- a/openrice_settings.xlsx
+++ b/openrice_settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hekal\Personal\Freelancing\Scrape_OpenRice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oiret\Downloads\OpenRice_Scraper_v1.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A29D9B7-B7BE-44D9-9B51-A983C27C7E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA147485-F984-4AAC-8338-77F92C54213E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openrice_settings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>New Restaurants</t>
   </si>
@@ -55,19 +55,16 @@
     <t>Restaurant Location</t>
   </si>
   <si>
-    <t>https://www.openrice.com/en/hongkong/r-gold-coast-prime-rib-tuen-mun-western-r491690</t>
-  </si>
-  <si>
-    <t>https://www.openrice.com/en/hongkong/r-moo-moo-kwun-tong-western-meatless-menu-r576967</t>
-  </si>
-  <si>
-    <t>tea</t>
-  </si>
-  <si>
-    <t>macau</t>
-  </si>
-  <si>
-    <t>Mikiki</t>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Kwun Tong</t>
+  </si>
+  <si>
+    <t>Causeway Bay</t>
   </si>
 </sst>
 </file>
@@ -922,26 +919,26 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -976,18 +973,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -996,34 +991,31 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{A3AB1F2A-438C-4A87-BA40-074994A26A23}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>